<commit_message>
Desmembrando o tratamento dos dados para que fique idependente
</commit_message>
<xml_diff>
--- a/data/baseTesteIXC.xlsx
+++ b/data/baseTesteIXC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weslley Carvalho\import_data_ixc\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94957B7E-52C4-409B-9703-ECB41D9C99AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7AC01D-E627-4C67-A7E8-55AD430E8A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8FC378E9-0372-46C3-819C-916EEC60C49E}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{8FC378E9-0372-46C3-819C-916EEC60C49E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -221,9 +221,6 @@
     <t>teste@gmail.com</t>
   </si>
   <si>
-    <t>194.327.600-57</t>
-  </si>
-  <si>
     <t>270.100.890-51</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>teste9@radios.com</t>
+  </si>
+  <si>
+    <t>835.212.320-34</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,7 +730,7 @@
         <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
         <v>25</v>
@@ -757,7 +757,7 @@
         <v>53</v>
       </c>
       <c r="P2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q2" t="s">
         <v>54</v>
@@ -777,7 +777,7 @@
         <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
@@ -804,7 +804,7 @@
         <v>53</v>
       </c>
       <c r="P3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q3" t="s">
         <v>55</v>
@@ -824,7 +824,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
@@ -851,7 +851,7 @@
         <v>53</v>
       </c>
       <c r="P4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q4" t="s">
         <v>56</v>
@@ -871,7 +871,7 @@
         <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>
@@ -898,7 +898,7 @@
         <v>53</v>
       </c>
       <c r="P5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q5" t="s">
         <v>55</v>
@@ -918,7 +918,7 @@
         <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
         <v>29</v>
@@ -942,7 +942,7 @@
         <v>53</v>
       </c>
       <c r="P6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q6" t="s">
         <v>57</v>
@@ -962,7 +962,7 @@
         <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
         <v>30</v>
@@ -989,7 +989,7 @@
         <v>53</v>
       </c>
       <c r="P7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q7" t="s">
         <v>55</v>
@@ -1009,7 +1009,7 @@
         <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
         <v>31</v>
@@ -1033,7 +1033,7 @@
         <v>53</v>
       </c>
       <c r="P8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q8" t="s">
         <v>55</v>
@@ -1053,7 +1053,7 @@
         <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
         <v>32</v>
@@ -1080,7 +1080,7 @@
         <v>53</v>
       </c>
       <c r="P9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q9" t="s">
         <v>55</v>
@@ -1100,7 +1100,7 @@
         <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
         <v>30</v>
@@ -1124,7 +1124,7 @@
         <v>53</v>
       </c>
       <c r="P10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q10" t="s">
         <v>55</v>

</xml_diff>